<commit_message>
Create match invoice API
</commit_message>
<xml_diff>
--- a/invoices/Sales RAW Data MPG-philips-2.xlsx
+++ b/invoices/Sales RAW Data MPG-philips-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
   <si>
     <t>Philips Lighting Sales By Category</t>
   </si>
@@ -67,9 +67,6 @@
     <t>26-10-2018</t>
   </si>
   <si>
-    <t>LI004461</t>
-  </si>
-  <si>
     <t>اسلام ابراهيم شخصى</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>LED Lamps</t>
+  </si>
+  <si>
+    <t>LI003092</t>
   </si>
 </sst>
 </file>
@@ -274,6 +274,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -286,35 +299,22 @@
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -779,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M14"/>
+  <dimension ref="B1:M13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="L6" sqref="L6:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -803,34 +803,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="53.85" customHeight="1">
-      <c r="B1" s="21"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B2" s="21"/>
-      <c r="G2" s="20" t="s">
+      <c r="B2" s="10"/>
+      <c r="G2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="2:13" ht="5.0999999999999996" customHeight="1"/>
     <row r="5" spans="2:13">
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="14"/>
       <c r="H5" s="1" t="s">
         <v>2</v>
@@ -844,173 +844,143 @@
       <c r="K5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M5" s="14"/>
     </row>
     <row r="6" spans="2:13">
-      <c r="D6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
+      <c r="D6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="13">
-        <v>1480</v>
+      <c r="L6" s="18">
+        <v>23</v>
       </c>
       <c r="M6" s="14"/>
     </row>
     <row r="7" spans="2:13">
-      <c r="D7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
+      <c r="D7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="13">
-        <v>2227</v>
+      <c r="L7" s="18">
+        <v>24</v>
       </c>
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="2:13" ht="15" customHeight="1">
-      <c r="D8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="13">
-        <v>3566</v>
+      <c r="L8" s="18">
+        <v>25</v>
       </c>
       <c r="M8" s="14"/>
     </row>
     <row r="9" spans="2:13" ht="15" customHeight="1">
-      <c r="D9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="13">
-        <v>1044</v>
+      <c r="L9" s="18">
+        <v>26</v>
       </c>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="2:13" ht="15" customHeight="1">
-      <c r="D10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="13">
-        <v>684</v>
-      </c>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="2:13" ht="18" customHeight="1">
-      <c r="D11" s="15" t="s">
+    <row r="10" spans="2:13" ht="18" customHeight="1">
+      <c r="D10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="15" t="s">
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="19">
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="24">
         <f>SUM(L6:M9)</f>
-        <v>8317</v>
-      </c>
-      <c r="M11" s="17"/>
-    </row>
-    <row r="12" spans="2:13" ht="4.5" customHeight="1"/>
-    <row r="13" spans="2:13" ht="18" customHeight="1">
-      <c r="B13" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="23"/>
+    </row>
+    <row r="11" spans="2:13" ht="4.5" customHeight="1"/>
+    <row r="12" spans="2:13" ht="18" customHeight="1">
+      <c r="B12" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="17"/>
-    </row>
-    <row r="14" spans="2:13" ht="15.95" customHeight="1"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="2:13" ht="15.95" customHeight="1"/>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G2:L3"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="H13:K13"/>
+  <mergeCells count="17">
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="D8:G8"/>
@@ -1018,10 +988,14 @@
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:K10"/>
     <mergeCell ref="L10:M10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G2:L3"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1055,34 +1029,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="53.85" customHeight="1">
-      <c r="B1" s="21"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="2:13" ht="12.2" customHeight="1">
-      <c r="B2" s="21"/>
-      <c r="G2" s="20" t="s">
+      <c r="B2" s="10"/>
+      <c r="G2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="2:13">
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
     </row>
     <row r="4" spans="2:13" ht="5.0999999999999996" customHeight="1"/>
     <row r="5" spans="2:13">
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="14"/>
       <c r="H5" s="1" t="s">
         <v>2</v>
@@ -1096,18 +1070,18 @@
       <c r="K5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="M5" s="14"/>
     </row>
     <row r="6" spans="2:13">
-      <c r="D6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
+      <c r="D6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1120,18 +1094,18 @@
       <c r="K6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="18">
         <v>480</v>
       </c>
       <c r="M6" s="14"/>
     </row>
     <row r="7" spans="2:13">
-      <c r="D7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
+      <c r="D7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1144,18 +1118,18 @@
       <c r="K7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="18">
         <v>1344</v>
       </c>
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="2:13">
-      <c r="D8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1168,18 +1142,18 @@
       <c r="K8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="18">
         <v>996</v>
       </c>
       <c r="M8" s="14"/>
     </row>
     <row r="9" spans="2:13">
-      <c r="D9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1192,18 +1166,18 @@
       <c r="K9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="18">
         <v>227.7</v>
       </c>
       <c r="M9" s="14"/>
     </row>
     <row r="10" spans="2:13">
-      <c r="D10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1216,18 +1190,18 @@
       <c r="K10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="18">
         <v>227.7</v>
       </c>
       <c r="M10" s="14"/>
     </row>
     <row r="11" spans="2:13">
-      <c r="D11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
+      <c r="D11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1240,18 +1214,18 @@
       <c r="K11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="18">
         <v>566.5</v>
       </c>
       <c r="M11" s="14"/>
     </row>
     <row r="12" spans="2:13">
-      <c r="D12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
+      <c r="D12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
       <c r="H12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1264,18 +1238,18 @@
       <c r="K12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="18">
         <v>1044</v>
       </c>
       <c r="M12" s="14"/>
     </row>
     <row r="13" spans="2:13" ht="15" customHeight="1">
-      <c r="D13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
+      <c r="D13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1288,63 +1262,45 @@
       <c r="K13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="18">
         <v>684.4</v>
       </c>
       <c r="M13" s="14"/>
     </row>
     <row r="14" spans="2:13" ht="18" customHeight="1">
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="15" t="s">
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="19">
+      <c r="I14" s="21"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="24">
         <f>SUM(L6:M12)</f>
         <v>4885.8999999999996</v>
       </c>
-      <c r="M14" s="17"/>
+      <c r="M14" s="23"/>
     </row>
     <row r="15" spans="2:13" ht="4.5" customHeight="1"/>
     <row r="16" spans="2:13" ht="18" customHeight="1">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="17"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" ht="15.95" customHeight="1"/>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G2:L3"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="L12:M12"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="L13:M13"/>
@@ -1352,6 +1308,24 @@
     <mergeCell ref="H14:K14"/>
     <mergeCell ref="L14:M14"/>
     <mergeCell ref="H16:K16"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G2:L3"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Latest changes for phase 2
</commit_message>
<xml_diff>
--- a/invoices/Sales RAW Data MPG-philips-2.xlsx
+++ b/invoices/Sales RAW Data MPG-philips-2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="20">
   <si>
     <t>Philips Lighting Sales By Category</t>
   </si>
@@ -74,12 +74,6 @@
   </si>
   <si>
     <t>Trade</t>
-  </si>
-  <si>
-    <t>SO-0017945</t>
-  </si>
-  <si>
-    <t>Lamps</t>
   </si>
   <si>
     <t>LED Lamps</t>
@@ -95,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-10409]#,##0.00;\(#,##0.00\)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -106,29 +100,34 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="22"/>
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -779,13 +778,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M13"/>
+  <dimension ref="B1:M10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:M9"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="5" customWidth="1"/>
@@ -802,10 +801,10 @@
     <col min="15" max="16384" width="8.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="53.85" customHeight="1">
+    <row r="1" spans="2:13" ht="53.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="2:13" ht="12.2" customHeight="1">
+    <row r="2" spans="2:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
       <c r="G2" s="11" t="s">
         <v>0</v>
@@ -816,7 +815,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -824,8 +823,8 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="2:13" ht="5.0999999999999996" customHeight="1"/>
-    <row r="5" spans="2:13">
+    <row r="4" spans="2:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
@@ -849,147 +848,69 @@
       </c>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D6" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
       <c r="H6" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>15</v>
       </c>
       <c r="L6" s="18">
-        <v>23</v>
+        <v>25000</v>
       </c>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="2:13">
-      <c r="D7" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="18">
-        <v>24</v>
-      </c>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="2:13" ht="15" customHeight="1">
-      <c r="D8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="18">
-        <v>25</v>
-      </c>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="2:13" ht="15" customHeight="1">
-      <c r="D9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="18">
-        <v>26</v>
-      </c>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="2:13" ht="18" customHeight="1">
-      <c r="D10" s="20" t="s">
+    <row r="7" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="20" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24">
-        <f>SUM(L6:M9)</f>
-        <v>98</v>
-      </c>
-      <c r="M10" s="23"/>
-    </row>
-    <row r="11" spans="2:13" ht="4.5" customHeight="1"/>
-    <row r="12" spans="2:13" ht="18" customHeight="1">
-      <c r="B12" s="19" t="s">
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="24">
+        <f>SUM(L6:M6)</f>
+        <v>25000</v>
+      </c>
+      <c r="M7" s="23"/>
+    </row>
+    <row r="8" spans="2:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
-    </row>
-    <row r="13" spans="2:13" ht="15.95" customHeight="1"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="H12:K12"/>
+  <mergeCells count="11">
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="H9:K9"/>
     <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:K7"/>
     <mergeCell ref="L7:M7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="G2:L3"/>
     <mergeCell ref="D5:G5"/>
@@ -1012,7 +933,7 @@
       <selection activeCell="L14" sqref="D2:M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
@@ -1028,10 +949,10 @@
     <col min="14" max="14" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="53.85" customHeight="1">
+    <row r="1" spans="2:13" ht="53.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="2:13" ht="12.2" customHeight="1">
+    <row r="2" spans="2:13" ht="12.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
       <c r="G2" s="11" t="s">
         <v>0</v>
@@ -1042,7 +963,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -1050,8 +971,8 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="2:13" ht="5.0999999999999996" customHeight="1"/>
-    <row r="5" spans="2:13">
+    <row r="4" spans="2:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1075,7 +996,7 @@
       </c>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D6" s="15" t="s">
         <v>17</v>
       </c>
@@ -1099,7 +1020,7 @@
       </c>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
@@ -1123,7 +1044,7 @@
       </c>
       <c r="M7" s="14"/>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D8" s="15" t="s">
         <v>17</v>
       </c>
@@ -1147,7 +1068,7 @@
       </c>
       <c r="M8" s="14"/>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D9" s="15" t="s">
         <v>17</v>
       </c>
@@ -1171,7 +1092,7 @@
       </c>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D10" s="15" t="s">
         <v>16</v>
       </c>
@@ -1195,7 +1116,7 @@
       </c>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D11" s="15" t="s">
         <v>16</v>
       </c>
@@ -1219,7 +1140,7 @@
       </c>
       <c r="M11" s="14"/>
     </row>
-    <row r="12" spans="2:13">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D12" s="15" t="s">
         <v>16</v>
       </c>
@@ -1243,7 +1164,7 @@
       </c>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="2:13" ht="15" customHeight="1">
+    <row r="13" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="15" t="s">
         <v>16</v>
       </c>
@@ -1267,7 +1188,7 @@
       </c>
       <c r="M13" s="14"/>
     </row>
-    <row r="14" spans="2:13" ht="18" customHeight="1">
+    <row r="14" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D14" s="20" t="s">
         <v>9</v>
       </c>
@@ -1286,8 +1207,8 @@
       </c>
       <c r="M14" s="23"/>
     </row>
-    <row r="15" spans="2:13" ht="4.5" customHeight="1"/>
-    <row r="16" spans="2:13" ht="18" customHeight="1">
+    <row r="15" spans="2:13" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
         <v>11</v>
       </c>
@@ -1298,7 +1219,7 @@
       <c r="J16" s="22"/>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" ht="15.95" customHeight="1"/>
+    <row r="17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
     <mergeCell ref="B16:D16"/>

</xml_diff>